<commit_message>
changed device count to 12
</commit_message>
<xml_diff>
--- a/examples/EMTF_MPCX_full/src/protocols.xlsx
+++ b/examples/EMTF_MPCX_full/src/protocols.xlsx
@@ -3558,13 +3558,13 @@
   <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
+      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="80.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.67"/>
   </cols>
@@ -3774,7 +3774,7 @@
         <v>50</v>
       </c>
       <c r="B20" s="1" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>51</v>

</xml_diff>

<commit_message>
fixed error in CPPF protocol, RXPCOMMAALIGNEN was 0, alignment did not work
</commit_message>
<xml_diff>
--- a/examples/EMTF_MPCX_full/src/protocols.xlsx
+++ b/examples/EMTF_MPCX_full/src/protocols.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="EMTF_root_config" sheetId="1" state="visible" r:id="rId2"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6420" uniqueCount="1124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6421" uniqueCount="1124">
   <si>
     <t xml:space="preserve">// path</t>
   </si>
@@ -3102,9 +3102,6 @@
     <t xml:space="preserve">rxmcommaalignen_in</t>
   </si>
   <si>
-    <t xml:space="preserve">rxpcommaalignen_in</t>
-  </si>
-  <si>
     <t xml:space="preserve">rxlpmhfhold_in</t>
   </si>
   <si>
@@ -3319,6 +3316,9 @@
   </si>
   <si>
     <t xml:space="preserve">TXOUTCLKSEL can also be selected to output TXOUTCLKPMA, which is automatically correct F for selected interface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RXPCOMMAALIGNEN should be set to 1 for 8b/10b protocols</t>
   </si>
   <si>
     <t xml:space="preserve">for COMMON modules:</t>
@@ -3575,7 +3575,7 @@
   </sheetPr>
   <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
     </sheetView>
   </sheetViews>
@@ -3910,7 +3910,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3942,7 +3942,7 @@
         <v>903</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4006,7 +4006,7 @@
         <v>914</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4100,7 +4100,7 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4132,7 +4132,7 @@
         <v>553</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4212,7 +4212,7 @@
         <v>545</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4260,7 +4260,7 @@
         <v>932</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4268,7 +4268,7 @@
         <v>934</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4316,7 +4316,7 @@
         <v>940</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4324,7 +4324,7 @@
         <v>942</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4356,7 +4356,7 @@
         <v>947</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4364,7 +4364,7 @@
         <v>949</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4372,7 +4372,7 @@
         <v>950</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4491,7 +4491,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4527,7 +4527,7 @@
         <v>967</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4604,7 +4604,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7041,7 +7041,7 @@
         <v>517</v>
       </c>
       <c r="B359" s="0" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="360" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7049,7 +7049,7 @@
         <v>519</v>
       </c>
       <c r="B360" s="0" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="361" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7057,7 +7057,7 @@
         <v>521</v>
       </c>
       <c r="B361" s="0" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="362" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7081,7 +7081,7 @@
         <v>526</v>
       </c>
       <c r="B364" s="0" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="365" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7097,7 +7097,7 @@
         <v>529</v>
       </c>
       <c r="B366" s="0" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="367" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7177,7 +7177,7 @@
         <v>543</v>
       </c>
       <c r="B376" s="0" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="377" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7185,7 +7185,7 @@
         <v>545</v>
       </c>
       <c r="B377" s="0" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="378" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7649,7 +7649,7 @@
         <v>621</v>
       </c>
       <c r="B435" s="0" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="436" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8169,7 +8169,7 @@
         <v>690</v>
       </c>
       <c r="B500" s="0" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="501" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8185,7 +8185,7 @@
         <v>693</v>
       </c>
       <c r="B502" s="0" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="503" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8257,7 +8257,7 @@
         <v>702</v>
       </c>
       <c r="B511" s="0" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="512" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8513,7 +8513,7 @@
         <v>737</v>
       </c>
       <c r="B543" s="0" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="544" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8521,7 +8521,7 @@
         <v>738</v>
       </c>
       <c r="B544" s="0" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="545" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8657,7 +8657,7 @@
         <v>755</v>
       </c>
       <c r="B561" s="0" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="562" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8665,7 +8665,7 @@
         <v>757</v>
       </c>
       <c r="B562" s="0" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="563" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8745,7 +8745,7 @@
         <v>766</v>
       </c>
       <c r="B572" s="0" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="573" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8889,7 +8889,7 @@
         <v>781</v>
       </c>
       <c r="B590" s="0" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="591" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8921,7 +8921,7 @@
         <v>784</v>
       </c>
       <c r="B594" s="0" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="595" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8937,7 +8937,7 @@
         <v>786</v>
       </c>
       <c r="B596" s="0" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="597" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9073,7 +9073,7 @@
         <v>803</v>
       </c>
       <c r="B613" s="0" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="614" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9089,7 +9089,7 @@
         <v>806</v>
       </c>
       <c r="B615" s="0" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="616" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9233,7 +9233,7 @@
         <v>823</v>
       </c>
       <c r="B633" s="0" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="634" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9241,7 +9241,7 @@
         <v>490</v>
       </c>
       <c r="B634" s="0" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="635" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9577,7 +9577,7 @@
         <v>863</v>
       </c>
       <c r="B676" s="0" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="677" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9585,7 +9585,7 @@
         <v>865</v>
       </c>
       <c r="B677" s="0" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="678" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9601,7 +9601,7 @@
         <v>868</v>
       </c>
       <c r="B679" s="0" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="680" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9609,7 +9609,7 @@
         <v>870</v>
       </c>
       <c r="B680" s="0" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="681" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9617,7 +9617,7 @@
         <v>872</v>
       </c>
       <c r="B681" s="0" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="682" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9697,7 +9697,7 @@
         <v>882</v>
       </c>
       <c r="B691" s="0" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="692" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9825,7 +9825,7 @@
         <v>894</v>
       </c>
       <c r="B707" s="0" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="708" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9885,7 +9885,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9906,10 +9906,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>1045</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>1046</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>1047</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9925,7 +9925,7 @@
         <v>903</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9989,7 +9989,7 @@
         <v>914</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10083,7 +10083,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10115,7 +10115,7 @@
         <v>553</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10195,7 +10195,7 @@
         <v>545</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10243,7 +10243,7 @@
         <v>932</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10251,7 +10251,7 @@
         <v>934</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10299,7 +10299,7 @@
         <v>940</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10307,7 +10307,7 @@
         <v>942</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10339,7 +10339,7 @@
         <v>947</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10347,7 +10347,7 @@
         <v>949</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10355,7 +10355,7 @@
         <v>950</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10474,7 +10474,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10501,7 +10501,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>59</v>
@@ -10510,7 +10510,7 @@
         <v>967</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10521,7 +10521,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>115</v>
@@ -10530,7 +10530,7 @@
         <v>967</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
   </sheetData>
@@ -10549,10 +10549,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10564,217 +10564,222 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="6" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="6" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="6" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="6" t="s">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="6" t="s">
         <v>1094</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="0" t="s">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="0" t="s">
         <v>1095</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="0" t="s">
-        <v>914</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>1096</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="0" t="s">
+        <v>914</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>1096</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" s="0" t="s">
         <v>917</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>1097</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
         <v>1098</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="0" t="s">
-        <v>1099</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="0" t="s">
         <v>1101</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C25" s="0" t="s">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C26" s="0" t="s">
         <v>1102</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="0" t="s">
-        <v>1103</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="0" t="s">
         <v>1104</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
         <v>1105</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="0" t="s">
-        <v>1106</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="0" t="s">
+        <v>1106</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="0" t="s">
         <v>1107</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="1" t="s">
-        <v>1108</v>
-      </c>
-      <c r="D32" s="0" t="s">
-        <v>1109</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="1" t="s">
-        <v>1110</v>
+        <v>1108</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>1111</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="1" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="1" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="1" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="1" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="1" t="s">
-        <v>1120</v>
+        <v>1118</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>1121</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="1" t="s">
+        <v>1120</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C40" s="1" t="s">
         <v>1122</v>
       </c>
-      <c r="D39" s="0" t="s">
+      <c r="D40" s="0" t="s">
         <v>1123</v>
       </c>
     </row>
@@ -18539,8 +18544,8 @@
   </sheetPr>
   <dimension ref="A1:J710"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A348" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A363" activeCellId="0" sqref="A363"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A459" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B484" activeCellId="0" sqref="B484"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -23606,7 +23611,7 @@
         <v>676</v>
       </c>
       <c r="B484" s="6" t="s">
-        <v>1022</v>
+        <v>524</v>
       </c>
       <c r="G484" s="4"/>
       <c r="H484" s="2"/>
@@ -23782,7 +23787,7 @@
         <v>690</v>
       </c>
       <c r="B500" s="6" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="G500" s="4"/>
       <c r="H500" s="2"/>
@@ -23804,7 +23809,7 @@
         <v>693</v>
       </c>
       <c r="B502" s="6" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="G502" s="4"/>
       <c r="H502" s="2"/>
@@ -24218,7 +24223,7 @@
         <v>737</v>
       </c>
       <c r="B543" s="6" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="544" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24226,7 +24231,7 @@
         <v>738</v>
       </c>
       <c r="B544" s="6" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="545" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24362,7 +24367,7 @@
         <v>755</v>
       </c>
       <c r="B561" s="6" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="562" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24370,7 +24375,7 @@
         <v>757</v>
       </c>
       <c r="B562" s="6" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="563" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24450,7 +24455,7 @@
         <v>766</v>
       </c>
       <c r="B572" s="6" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="573" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24570,7 +24575,7 @@
         <v>777</v>
       </c>
       <c r="B587" s="6" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="588" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24594,7 +24599,7 @@
         <v>781</v>
       </c>
       <c r="B590" s="6" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="591" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24626,7 +24631,7 @@
         <v>784</v>
       </c>
       <c r="B594" s="6" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="595" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24642,7 +24647,7 @@
         <v>786</v>
       </c>
       <c r="B596" s="6" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="597" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24778,7 +24783,7 @@
         <v>803</v>
       </c>
       <c r="B613" s="6" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="614" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24794,7 +24799,7 @@
         <v>806</v>
       </c>
       <c r="B615" s="6" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="616" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24938,7 +24943,7 @@
         <v>823</v>
       </c>
       <c r="B633" s="6" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="634" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24946,7 +24951,7 @@
         <v>490</v>
       </c>
       <c r="B634" s="6" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="635" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25282,7 +25287,7 @@
         <v>863</v>
       </c>
       <c r="B676" s="6" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="677" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25290,7 +25295,7 @@
         <v>865</v>
       </c>
       <c r="B677" s="6" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="678" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25306,7 +25311,7 @@
         <v>868</v>
       </c>
       <c r="B679" s="6" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="680" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25314,7 +25319,7 @@
         <v>870</v>
       </c>
       <c r="B680" s="6" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="681" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25322,7 +25327,7 @@
         <v>872</v>
       </c>
       <c r="B681" s="6" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="682" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25402,7 +25407,7 @@
         <v>882</v>
       </c>
       <c r="B691" s="6" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="692" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25466,7 +25471,7 @@
         <v>889</v>
       </c>
       <c r="B699" s="6" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="700" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25530,7 +25535,7 @@
         <v>894</v>
       </c>
       <c r="B707" s="6" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="708" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25611,10 +25616,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>1045</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>1046</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>1047</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25630,7 +25635,7 @@
         <v>903</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25694,7 +25699,7 @@
         <v>914</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25788,7 +25793,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25822,7 +25827,7 @@
         <v>553</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="D33" s="4"/>
     </row>
@@ -25909,7 +25914,7 @@
         <v>545</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="D43" s="4"/>
     </row>
@@ -25962,7 +25967,7 @@
         <v>932</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="D49" s="4"/>
     </row>
@@ -25971,7 +25976,7 @@
         <v>934</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="D50" s="4"/>
     </row>
@@ -26020,7 +26025,7 @@
         <v>940</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="D56" s="4"/>
     </row>
@@ -26029,7 +26034,7 @@
         <v>942</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26063,7 +26068,7 @@
         <v>947</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26071,7 +26076,7 @@
         <v>949</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="D62" s="4"/>
     </row>
@@ -26080,7 +26085,7 @@
         <v>950</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26228,7 +26233,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>59</v>
@@ -26237,7 +26242,7 @@
         <v>967</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26248,7 +26253,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>115</v>
@@ -26257,7 +26262,7 @@
         <v>967</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
   </sheetData>
@@ -26294,7 +26299,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26315,7 +26320,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26467,7 +26472,7 @@
         <v>147</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29344,7 +29349,7 @@
         <v>621</v>
       </c>
       <c r="B436" s="0" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="437" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29864,7 +29869,7 @@
         <v>690</v>
       </c>
       <c r="B501" s="0" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="502" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29880,7 +29885,7 @@
         <v>693</v>
       </c>
       <c r="B503" s="0" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="504" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30208,7 +30213,7 @@
         <v>737</v>
       </c>
       <c r="B544" s="0" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="545" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30216,7 +30221,7 @@
         <v>738</v>
       </c>
       <c r="B545" s="0" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="546" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30352,7 +30357,7 @@
         <v>755</v>
       </c>
       <c r="B562" s="0" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="563" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30360,7 +30365,7 @@
         <v>757</v>
       </c>
       <c r="B563" s="0" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="564" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30440,7 +30445,7 @@
         <v>766</v>
       </c>
       <c r="B573" s="0" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="574" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30560,7 +30565,7 @@
         <v>777</v>
       </c>
       <c r="B588" s="0" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="589" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30584,7 +30589,7 @@
         <v>781</v>
       </c>
       <c r="B591" s="0" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="592" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30616,7 +30621,7 @@
         <v>784</v>
       </c>
       <c r="B595" s="0" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="596" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30632,7 +30637,7 @@
         <v>786</v>
       </c>
       <c r="B597" s="0" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="598" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30768,7 +30773,7 @@
         <v>803</v>
       </c>
       <c r="B614" s="0" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="615" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30784,7 +30789,7 @@
         <v>806</v>
       </c>
       <c r="B616" s="0" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="617" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30928,7 +30933,7 @@
         <v>823</v>
       </c>
       <c r="B634" s="0" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="635" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30936,7 +30941,7 @@
         <v>490</v>
       </c>
       <c r="B635" s="0" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="636" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31272,7 +31277,7 @@
         <v>863</v>
       </c>
       <c r="B677" s="0" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="678" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31280,7 +31285,7 @@
         <v>865</v>
       </c>
       <c r="B678" s="0" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="679" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31296,7 +31301,7 @@
         <v>868</v>
       </c>
       <c r="B680" s="0" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="681" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31304,7 +31309,7 @@
         <v>870</v>
       </c>
       <c r="B681" s="0" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="682" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31312,7 +31317,7 @@
         <v>872</v>
       </c>
       <c r="B682" s="0" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="683" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31392,7 +31397,7 @@
         <v>882</v>
       </c>
       <c r="B692" s="0" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="693" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31456,7 +31461,7 @@
         <v>889</v>
       </c>
       <c r="B700" s="0" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="701" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>